<commit_message>
Update AuditRowUpdaterServiceTests for new UT config and profile.
</commit_message>
<xml_diff>
--- a/src/test/resources/integration/IntegrationTest-ExpectedResults.xlsx
+++ b/src/test/resources/integration/IntegrationTest-ExpectedResults.xlsx
@@ -4,18 +4,18 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="40" yWindow="12940" windowWidth="32000" windowHeight="5530" tabRatio="707" firstSheet="2" activeTab="3"/>
+    <workbookView xWindow="-80" yWindow="90" windowWidth="37900" windowHeight="2910" tabRatio="707" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="Vendor Not Found" sheetId="14" r:id="rId1"/>
     <sheet name="Microsoft" sheetId="2" r:id="rId2"/>
-    <sheet name="Cisco Systems, Inc." sheetId="1" r:id="rId3"/>
-    <sheet name="Fortinet Technologies Inc" sheetId="3" r:id="rId4"/>
+    <sheet name="CISCO" sheetId="1" r:id="rId3"/>
+    <sheet name="Fortinet Technologies" sheetId="3" r:id="rId4"/>
     <sheet name="Citrix" sheetId="13" r:id="rId5"/>
-    <sheet name="Oracle Corporation" sheetId="4" r:id="rId6"/>
+    <sheet name="Oracle" sheetId="4" r:id="rId6"/>
     <sheet name="Test Vendor 1" sheetId="5" r:id="rId7"/>
     <sheet name="Test Vendor 2" sheetId="6" r:id="rId8"/>
-    <sheet name="Waves Audio Ltd." sheetId="7" r:id="rId9"/>
+    <sheet name="Waves Audio" sheetId="7" r:id="rId9"/>
     <sheet name="CheckPoint" sheetId="8" r:id="rId10"/>
     <sheet name="Adobe" sheetId="9" r:id="rId11"/>
     <sheet name="Business Objects" sheetId="10" r:id="rId12"/>
@@ -942,8 +942,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="43.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1086,7 +1086,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="41.26953125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1151,7 +1151,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
@@ -1497,7 +1497,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E2"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Add RowNumber to get the next row number in a sheet.
</commit_message>
<xml_diff>
--- a/src/test/resources/integration/IntegrationTest-ExpectedResults.xlsx
+++ b/src/test/resources/integration/IntegrationTest-ExpectedResults.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-80" yWindow="90" windowWidth="37900" windowHeight="2910" tabRatio="707" activeTab="13"/>
+    <workbookView xWindow="-80" yWindow="90" windowWidth="36730" windowHeight="13740" tabRatio="707" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="Vendor Not Found" sheetId="14" r:id="rId1"/>
@@ -53,18 +53,12 @@
     <t>{C2324E3B-0AED-4413-82FA-F638913C264A}</t>
   </si>
   <si>
-    <t>CISC_C2324E3B</t>
-  </si>
-  <si>
     <t>Cisco AnyConnect Secure Mobility Client</t>
   </si>
   <si>
     <t>4.9.01095</t>
   </si>
   <si>
-    <t>MS_90120000</t>
-  </si>
-  <si>
     <t>6.0.7.0243</t>
   </si>
   <si>
@@ -83,21 +77,12 @@
     <t>Citrix Workspace(DV)</t>
   </si>
   <si>
-    <t>CTRX_BD45A07E</t>
-  </si>
-  <si>
-    <t>FRT_FE1638FD</t>
-  </si>
-  <si>
     <t>Citrix Authentication Manager</t>
   </si>
   <si>
     <t>{8CA6F29E-DF02-4519-B33C-9AC9935D28D9}</t>
   </si>
   <si>
-    <t>CTRX_8CA6F29E</t>
-  </si>
-  <si>
     <t>20.11.0.12</t>
   </si>
   <si>
@@ -107,15 +92,9 @@
     <t>{8CA6F29E-DF02-4519-B33C-9AC9935D28E9}</t>
   </si>
   <si>
-    <t>CTRX_8CA6F29E_1</t>
-  </si>
-  <si>
     <t>{2E72FA1F-BADB-4337-B8AE-F7C17EC57D1D}</t>
   </si>
   <si>
-    <t>MS_2E72FA1F</t>
-  </si>
-  <si>
     <t>Microsoft Visual C++ 2019 X86 Minimum Runtime - 14.24.28127</t>
   </si>
   <si>
@@ -131,18 +110,12 @@
     <t>{4A03706F-666A-4037-7777-5F2748764D10}</t>
   </si>
   <si>
-    <t>ORC_4A03706F</t>
-  </si>
-  <si>
     <t>PHP Manager 1.4 for IIS 10</t>
   </si>
   <si>
     <t>{E851486F-1FE2-44F0-85ED-F969088A68EE}</t>
   </si>
   <si>
-    <t>VNF_E851486F</t>
-  </si>
-  <si>
     <t>1.4.0</t>
   </si>
   <si>
@@ -152,9 +125,6 @@
     <t>1.0.2.2</t>
   </si>
   <si>
-    <t>TV1_E851486F</t>
-  </si>
-  <si>
     <t>9.4.5</t>
   </si>
   <si>
@@ -164,9 +134,6 @@
     <t>{4A03706F-666A-4037-9177-5F2748764D10}</t>
   </si>
   <si>
-    <t>TV2_4A03706F</t>
-  </si>
-  <si>
     <t>Installed Asset IDs</t>
   </si>
   <si>
@@ -188,9 +155,6 @@
     <t>Maxx Audio Installer (x64)</t>
   </si>
   <si>
-    <t>WVS_307032B2</t>
-  </si>
-  <si>
     <t>{22123B83-0475-4A1C-B658-CDAA196486F2}</t>
   </si>
   <si>
@@ -200,9 +164,6 @@
     <t>20.12.0.10</t>
   </si>
   <si>
-    <t>CTRX_22123B83</t>
-  </si>
-  <si>
     <t>{4D38C3A3-B685-4AB5-BD6D-FD88BCED5805}</t>
   </si>
   <si>
@@ -212,15 +173,9 @@
     <t>5.1.51515.0</t>
   </si>
   <si>
-    <t>MS_4D38C3A3</t>
-  </si>
-  <si>
     <t>{26A24AE4-039D-4CA4-87B4-2F32180231F0}</t>
   </si>
   <si>
-    <t>ORC_26A24AE4</t>
-  </si>
-  <si>
     <t>Java 8 Update 231</t>
   </si>
   <si>
@@ -236,9 +191,6 @@
     <t>Check Point SSL Network Extender Service</t>
   </si>
   <si>
-    <t>CHKP_588ec085</t>
-  </si>
-  <si>
     <t>22.002.20191</t>
   </si>
   <si>
@@ -248,9 +200,6 @@
     <t>Adobe Acrobat Reader DC</t>
   </si>
   <si>
-    <t>ADBE_AC76BA86</t>
-  </si>
-  <si>
     <t>{4D46B3A6-67F5-4385-86D2-8E769EA07827}</t>
   </si>
   <si>
@@ -260,9 +209,6 @@
     <t>19.11.100.48</t>
   </si>
   <si>
-    <t>CTRX_4D46B3A6</t>
-  </si>
-  <si>
     <t>98.61.1703</t>
   </si>
   <si>
@@ -272,9 +218,6 @@
     <t>{5E867838-8E7D-4B0D-8D7F-46698BC6414D}</t>
   </si>
   <si>
-    <t>CHKP_5E867838</t>
-  </si>
-  <si>
     <t>11.5.0.31327</t>
   </si>
   <si>
@@ -284,9 +227,6 @@
     <t>Crystal Reports XI Release 2</t>
   </si>
   <si>
-    <t>BOBJ_94FB0978</t>
-  </si>
-  <si>
     <t>20.3.1</t>
   </si>
   <si>
@@ -296,9 +236,6 @@
     <t>{836AC60A-957F-49A2-9235-2538FB2B490F}</t>
   </si>
   <si>
-    <t>CNWS_836AC60A</t>
-  </si>
-  <si>
     <t>{90B2724A-9C22-4C6C-B111-5D21E348ADF3}</t>
   </si>
   <si>
@@ -308,9 +245,6 @@
     <t>39.9.2.116</t>
   </si>
   <si>
-    <t>CISC_90B2724A</t>
-  </si>
-  <si>
     <t>13.0.15.1840</t>
   </si>
   <si>
@@ -320,7 +254,73 @@
     <t>{8055CFEA-3871-4C76-A321-E32F63637CC4}</t>
   </si>
   <si>
-    <t>SAP_8055CFEA</t>
+    <t>VNF_1</t>
+  </si>
+  <si>
+    <t>MS_1</t>
+  </si>
+  <si>
+    <t>MS_2</t>
+  </si>
+  <si>
+    <t>MS_3</t>
+  </si>
+  <si>
+    <t>FT_1</t>
+  </si>
+  <si>
+    <t>CTRX_1</t>
+  </si>
+  <si>
+    <t>CTRX_2</t>
+  </si>
+  <si>
+    <t>CTRX_3</t>
+  </si>
+  <si>
+    <t>CTRX_4</t>
+  </si>
+  <si>
+    <t>CTRX_5</t>
+  </si>
+  <si>
+    <t>ORC_1</t>
+  </si>
+  <si>
+    <t>ORC_2</t>
+  </si>
+  <si>
+    <t>TV_1</t>
+  </si>
+  <si>
+    <t>TV_2</t>
+  </si>
+  <si>
+    <t>CP_1</t>
+  </si>
+  <si>
+    <t>CP_2</t>
+  </si>
+  <si>
+    <t>ADOBE_1</t>
+  </si>
+  <si>
+    <t>CISCO_1</t>
+  </si>
+  <si>
+    <t>CISCO_2</t>
+  </si>
+  <si>
+    <t>WAVES_1</t>
+  </si>
+  <si>
+    <t>BO_1</t>
+  </si>
+  <si>
+    <t>CW_1</t>
+  </si>
+  <si>
+    <t>SAP_1</t>
   </si>
 </sst>
 </file>
@@ -662,7 +662,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E2"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="26.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -687,24 +687,24 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>37</v>
+        <v>75</v>
       </c>
       <c r="B2" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="C2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E2" t="s">
         <v>36</v>
-      </c>
-      <c r="D2" t="s">
-        <v>38</v>
-      </c>
-      <c r="E2" t="s">
-        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -717,7 +717,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="A2" sqref="A2:A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="25.26953125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -739,41 +739,41 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>69</v>
+        <v>89</v>
       </c>
       <c r="B2" t="s">
-        <v>68</v>
+        <v>53</v>
       </c>
       <c r="C2" t="s">
-        <v>67</v>
+        <v>52</v>
       </c>
       <c r="D2" t="s">
-        <v>66</v>
+        <v>51</v>
       </c>
       <c r="E2" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="B3" t="s">
-        <v>79</v>
+        <v>61</v>
       </c>
       <c r="C3" t="s">
-        <v>80</v>
+        <v>62</v>
       </c>
       <c r="D3" t="s">
-        <v>78</v>
+        <v>60</v>
       </c>
       <c r="E3" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -786,7 +786,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E2"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="25.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -805,24 +805,24 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>73</v>
+        <v>91</v>
       </c>
       <c r="B2" t="s">
-        <v>72</v>
+        <v>56</v>
       </c>
       <c r="C2" t="s">
-        <v>71</v>
+        <v>55</v>
       </c>
       <c r="D2" t="s">
-        <v>70</v>
+        <v>54</v>
       </c>
       <c r="E2" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -835,7 +835,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -857,24 +857,24 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>85</v>
+        <v>95</v>
       </c>
       <c r="B2" t="s">
-        <v>84</v>
+        <v>65</v>
       </c>
       <c r="C2" t="s">
-        <v>83</v>
+        <v>64</v>
       </c>
       <c r="D2" t="s">
-        <v>82</v>
+        <v>63</v>
       </c>
       <c r="E2" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -887,7 +887,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -913,24 +913,24 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>89</v>
+        <v>96</v>
       </c>
       <c r="B2" t="s">
-        <v>87</v>
+        <v>67</v>
       </c>
       <c r="C2" t="s">
-        <v>88</v>
+        <v>68</v>
       </c>
       <c r="D2" t="s">
-        <v>86</v>
+        <v>66</v>
       </c>
       <c r="E2" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -943,7 +943,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="43.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -967,7 +967,7 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
@@ -975,16 +975,16 @@
         <v>97</v>
       </c>
       <c r="B2" t="s">
-        <v>95</v>
+        <v>73</v>
       </c>
       <c r="C2" t="s">
-        <v>96</v>
+        <v>74</v>
       </c>
       <c r="D2" t="s">
-        <v>94</v>
+        <v>72</v>
       </c>
       <c r="E2" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -997,7 +997,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="A2" sqref="A2:A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="21.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1022,12 +1022,12 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>76</v>
       </c>
       <c r="B2" t="s">
         <v>5</v>
@@ -1039,41 +1039,41 @@
         <v>6</v>
       </c>
       <c r="E2" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>28</v>
+        <v>77</v>
       </c>
       <c r="B3" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="C3" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="D3" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="E3" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>61</v>
+        <v>78</v>
       </c>
       <c r="B4" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
       <c r="C4" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="D4" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="E4" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -1086,7 +1086,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="A2" sqref="A2:A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="41.26953125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1105,24 +1105,24 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B2" t="s">
         <v>8</v>
-      </c>
-      <c r="B2" t="s">
-        <v>9</v>
       </c>
       <c r="C2" t="s">
         <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
@@ -1130,16 +1130,16 @@
         <v>93</v>
       </c>
       <c r="B3" t="s">
-        <v>91</v>
+        <v>70</v>
       </c>
       <c r="C3" t="s">
-        <v>90</v>
+        <v>69</v>
       </c>
       <c r="D3" t="s">
-        <v>92</v>
+        <v>71</v>
       </c>
       <c r="E3" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -1152,7 +1152,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="43.26953125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1171,24 +1171,24 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>19</v>
+        <v>79</v>
       </c>
       <c r="B2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E2" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -1223,92 +1223,92 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>18</v>
+        <v>80</v>
       </c>
       <c r="B2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>22</v>
+        <v>81</v>
       </c>
       <c r="B3" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C3" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="D3" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="E3" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>26</v>
+        <v>82</v>
       </c>
       <c r="B4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" t="s">
         <v>20</v>
       </c>
-      <c r="C4" t="s">
-        <v>25</v>
-      </c>
       <c r="D4" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="E4" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>57</v>
+        <v>83</v>
       </c>
       <c r="B5" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="C5" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="D5" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="E5" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="B6" t="s">
-        <v>75</v>
+        <v>58</v>
       </c>
       <c r="C6" t="s">
-        <v>74</v>
+        <v>57</v>
       </c>
       <c r="D6" t="s">
-        <v>76</v>
+        <v>59</v>
       </c>
       <c r="E6" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -1321,7 +1321,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="27.6328125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1343,41 +1343,41 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>34</v>
+        <v>85</v>
       </c>
       <c r="B2" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="C2" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="D2" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="E2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>63</v>
+        <v>86</v>
       </c>
       <c r="B3" t="s">
-        <v>64</v>
+        <v>49</v>
       </c>
       <c r="C3" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
       <c r="D3" t="s">
-        <v>65</v>
+        <v>50</v>
       </c>
       <c r="E3" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -1390,7 +1390,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E2"/>
+      <selection activeCell="E41" sqref="E41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1412,24 +1412,24 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>41</v>
+        <v>87</v>
       </c>
       <c r="B2" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="C2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E2" t="s">
         <v>36</v>
-      </c>
-      <c r="D2" t="s">
-        <v>40</v>
-      </c>
-      <c r="E2" t="s">
-        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -1442,7 +1442,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1467,24 +1467,24 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>45</v>
+        <v>88</v>
       </c>
       <c r="B2" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="C2" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="D2" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="E2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -1497,7 +1497,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1523,24 +1523,24 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>53</v>
+        <v>94</v>
       </c>
       <c r="B2" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="C2" t="s">
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="D2" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="E2" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Change Asset ID to be host name only.
</commit_message>
<xml_diff>
--- a/src/test/resources/integration/IntegrationTest-ExpectedResults.xlsx
+++ b/src/test/resources/integration/IntegrationTest-ExpectedResults.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-80" yWindow="90" windowWidth="36730" windowHeight="13740" tabRatio="707" activeTab="13"/>
+    <workbookView xWindow="-80" yWindow="6380" windowWidth="36730" windowHeight="7450" tabRatio="707" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="Vendor Not Found" sheetId="14" r:id="rId1"/>
@@ -137,15 +137,6 @@
     <t>Installed Asset IDs</t>
   </si>
   <si>
-    <t>IntTestBadApps_Bad-Apps;</t>
-  </si>
-  <si>
-    <t>IntTestGoodApps_Good-Apps;</t>
-  </si>
-  <si>
-    <t>IntTestBadApps_Bad-Apps;IntTestGoodApps_Good-Apps;</t>
-  </si>
-  <si>
     <t>{307032B2-6AF2-46D7-B933-62438DEB2B9A}</t>
   </si>
   <si>
@@ -290,12 +281,6 @@
     <t>ORC_2</t>
   </si>
   <si>
-    <t>TV_1</t>
-  </si>
-  <si>
-    <t>TV_2</t>
-  </si>
-  <si>
     <t>CP_1</t>
   </si>
   <si>
@@ -321,6 +306,21 @@
   </si>
   <si>
     <t>SAP_1</t>
+  </si>
+  <si>
+    <t>Good-Apps;</t>
+  </si>
+  <si>
+    <t>Bad-Apps;</t>
+  </si>
+  <si>
+    <t>Bad-Apps;Good-Apps;</t>
+  </si>
+  <si>
+    <t>TV1_1</t>
+  </si>
+  <si>
+    <t>TV2_1</t>
   </si>
 </sst>
 </file>
@@ -662,7 +662,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="26.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -692,7 +692,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B2" t="s">
         <v>27</v>
@@ -704,7 +704,7 @@
         <v>29</v>
       </c>
       <c r="E2" t="s">
-        <v>36</v>
+        <v>94</v>
       </c>
     </row>
   </sheetData>
@@ -744,36 +744,36 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="B2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C2" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D2" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E2" t="s">
-        <v>37</v>
+        <v>93</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="B3" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C3" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D3" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E3" t="s">
-        <v>37</v>
+        <v>93</v>
       </c>
     </row>
   </sheetData>
@@ -810,19 +810,19 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="B2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C2" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D2" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="E2" t="s">
-        <v>37</v>
+        <v>93</v>
       </c>
     </row>
   </sheetData>
@@ -862,19 +862,19 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="B2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C2" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D2" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E2" t="s">
-        <v>37</v>
+        <v>93</v>
       </c>
     </row>
   </sheetData>
@@ -918,19 +918,19 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="B2" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="E2" t="s">
-        <v>37</v>
+        <v>93</v>
       </c>
     </row>
   </sheetData>
@@ -943,7 +943,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="43.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -972,19 +972,19 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="B2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="D2" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="E2" t="s">
-        <v>37</v>
+        <v>93</v>
       </c>
     </row>
   </sheetData>
@@ -997,7 +997,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A4"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="21.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1027,7 +1027,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B2" t="s">
         <v>5</v>
@@ -1039,12 +1039,12 @@
         <v>6</v>
       </c>
       <c r="E2" t="s">
-        <v>38</v>
+        <v>95</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B3" t="s">
         <v>22</v>
@@ -1056,24 +1056,24 @@
         <v>23</v>
       </c>
       <c r="E3" t="s">
-        <v>36</v>
+        <v>94</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B4" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C4" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D4" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="E4" t="s">
-        <v>37</v>
+        <v>93</v>
       </c>
     </row>
   </sheetData>
@@ -1086,7 +1086,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A3"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="41.26953125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1110,7 +1110,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="B2" t="s">
         <v>8</v>
@@ -1122,24 +1122,24 @@
         <v>9</v>
       </c>
       <c r="E2" t="s">
-        <v>36</v>
+        <v>94</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
+        <v>88</v>
+      </c>
+      <c r="B3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D3" t="s">
+        <v>68</v>
+      </c>
+      <c r="E3" t="s">
         <v>93</v>
-      </c>
-      <c r="B3" t="s">
-        <v>70</v>
-      </c>
-      <c r="C3" t="s">
-        <v>69</v>
-      </c>
-      <c r="D3" t="s">
-        <v>71</v>
-      </c>
-      <c r="E3" t="s">
-        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -1152,7 +1152,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="43.26953125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1176,7 +1176,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B2" t="s">
         <v>11</v>
@@ -1188,7 +1188,7 @@
         <v>10</v>
       </c>
       <c r="E2" t="s">
-        <v>38</v>
+        <v>95</v>
       </c>
     </row>
   </sheetData>
@@ -1201,7 +1201,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="30.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1228,7 +1228,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B2" t="s">
         <v>15</v>
@@ -1240,12 +1240,12 @@
         <v>14</v>
       </c>
       <c r="E2" t="s">
-        <v>36</v>
+        <v>94</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B3" t="s">
         <v>16</v>
@@ -1257,12 +1257,12 @@
         <v>18</v>
       </c>
       <c r="E3" t="s">
-        <v>36</v>
+        <v>94</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B4" t="s">
         <v>16</v>
@@ -1274,41 +1274,41 @@
         <v>19</v>
       </c>
       <c r="E4" t="s">
-        <v>36</v>
+        <v>94</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B5" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C5" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D5" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E5" t="s">
-        <v>37</v>
+        <v>93</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B6" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C6" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D6" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="E6" t="s">
-        <v>37</v>
+        <v>93</v>
       </c>
     </row>
   </sheetData>
@@ -1348,7 +1348,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B2" t="s">
         <v>25</v>
@@ -1360,24 +1360,24 @@
         <v>24</v>
       </c>
       <c r="E2" t="s">
-        <v>36</v>
+        <v>94</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C3" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D3" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E3" t="s">
-        <v>37</v>
+        <v>93</v>
       </c>
     </row>
   </sheetData>
@@ -1390,7 +1390,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E41" sqref="E41"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1417,7 +1417,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>87</v>
+        <v>96</v>
       </c>
       <c r="B2" t="s">
         <v>30</v>
@@ -1429,7 +1429,7 @@
         <v>31</v>
       </c>
       <c r="E2" t="s">
-        <v>36</v>
+        <v>94</v>
       </c>
     </row>
   </sheetData>
@@ -1442,7 +1442,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1472,7 +1472,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>88</v>
+        <v>97</v>
       </c>
       <c r="B2" t="s">
         <v>33</v>
@@ -1484,7 +1484,7 @@
         <v>32</v>
       </c>
       <c r="E2" t="s">
-        <v>36</v>
+        <v>94</v>
       </c>
     </row>
   </sheetData>
@@ -1528,19 +1528,19 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="B2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E2" t="s">
-        <v>37</v>
+        <v>93</v>
       </c>
     </row>
   </sheetData>

</xml_diff>